<commit_message>
Move sord sampe out from dataset.
</commit_message>
<xml_diff>
--- a/relations_entity_distance.xlsx
+++ b/relations_entity_distance.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0A0E40-FF20-4D8D-A497-92777E5CD70D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8F73AC-15ED-4531-9EF9-8C5261B495D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Entity Ditance</t>
+    <t>Relation Numbel</t>
   </si>
   <si>
-    <t>Relation Numbel</t>
+    <t>Entity Distance</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="B1:C832"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,10 +442,10 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>